<commit_message>
Adding a Review about HLD
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.1.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
   <si>
     <t>Review Log</t>
   </si>
@@ -464,11 +464,23 @@
       <t>you didn’t mention power supply and switch</t>
     </r>
   </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>RAMADAN</t>
+  </si>
+  <si>
+    <t>Mostafa</t>
+  </si>
+  <si>
+    <t>You should put the HLD In a Word file with a a describation  for it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,7 +535,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,6 +545,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEA9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,9 +800,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,6 +812,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -824,21 +860,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,9 +1173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,22 +1234,22 @@
       <c r="B2" s="4">
         <v>1.2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="43">
         <v>2</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="43" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -1237,12 +1265,12 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1256,12 +1284,12 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1275,12 +1303,12 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1294,12 +1322,12 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1313,12 +1341,12 @@
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1332,12 +1360,12 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1351,12 +1379,12 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1370,12 +1398,12 @@
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
       <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1389,12 +1417,12 @@
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="16" t="s">
         <v>28</v>
       </c>
@@ -1408,12 +1436,12 @@
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1427,12 +1455,12 @@
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1446,12 +1474,12 @@
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1465,12 +1493,12 @@
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1484,12 +1512,12 @@
       <c r="B16" s="7">
         <v>2.5</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1565,31 +1593,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="43">
         <v>1</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="43" t="s">
         <v>41</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="49" t="s">
+      <c r="J19" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="46" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1598,17 +1626,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="41"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="47"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -1617,17 +1645,17 @@
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="41"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -1636,17 +1664,17 @@
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="50"/>
-      <c r="K22" s="41"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -1655,17 +1683,17 @@
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="50"/>
-      <c r="K23" s="41"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="47"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1674,17 +1702,17 @@
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="50"/>
-      <c r="K24" s="41"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1693,17 +1721,17 @@
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="50"/>
-      <c r="K25" s="41"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1712,34 +1740,34 @@
       <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="50"/>
-      <c r="K26" s="41"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="50"/>
-      <c r="K27" s="41"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="47"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1748,17 +1776,17 @@
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="50"/>
-      <c r="K28" s="41"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="47"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1767,17 +1795,17 @@
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="50"/>
-      <c r="K29" s="41"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1786,17 +1814,17 @@
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="50"/>
-      <c r="K30" s="41"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="47"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -1805,17 +1833,17 @@
       <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="41"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="47"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -1824,17 +1852,17 @@
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
       <c r="I32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="50"/>
-      <c r="K32" s="41"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="47"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1843,17 +1871,17 @@
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
       <c r="I33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J33" s="50"/>
-      <c r="K33" s="41"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="47"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
@@ -1862,17 +1890,17 @@
       <c r="B34" s="7">
         <v>6.2</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
       <c r="I34" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="51"/>
-      <c r="K34" s="42"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="48"/>
     </row>
     <row r="35" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31">
@@ -1881,20 +1909,20 @@
       <c r="B35" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="52" t="s">
         <v>71</v>
       </c>
       <c r="E35" s="11"/>
-      <c r="F35" s="43" t="s">
+      <c r="F35" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="43" t="s">
+      <c r="G35" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="49" t="s">
+      <c r="H35" s="43" t="s">
         <v>73</v>
       </c>
       <c r="I35" s="32" t="s">
@@ -1914,12 +1942,12 @@
       <c r="B36" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="47"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="44"/>
       <c r="I36" s="33" t="s">
         <v>75</v>
       </c>
@@ -1937,12 +1965,12 @@
       <c r="B37" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="13"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="44"/>
       <c r="I37" s="33" t="s">
         <v>76</v>
       </c>
@@ -1963,12 +1991,12 @@
       <c r="B38" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="47"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="13"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="44"/>
       <c r="I38" s="33" t="s">
         <v>78</v>
       </c>
@@ -1986,12 +2014,12 @@
       <c r="B39" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="47"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="44"/>
       <c r="I39" s="33" t="s">
         <v>75</v>
       </c>
@@ -2009,12 +2037,12 @@
       <c r="B40" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="47"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="44"/>
       <c r="I40" s="33" t="s">
         <v>76</v>
       </c>
@@ -2035,12 +2063,12 @@
       <c r="B41" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="47"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="44"/>
       <c r="I41" s="33" t="s">
         <v>75</v>
       </c>
@@ -2058,12 +2086,12 @@
       <c r="B42" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="47"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="44"/>
       <c r="I42" s="33" t="s">
         <v>76</v>
       </c>
@@ -2084,12 +2112,12 @@
       <c r="B43" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="47"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="44"/>
       <c r="I43" s="33" t="s">
         <v>75</v>
       </c>
@@ -2107,12 +2135,12 @@
       <c r="B44" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="47"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="44"/>
       <c r="I44" s="33" t="s">
         <v>81</v>
       </c>
@@ -2133,12 +2161,12 @@
       <c r="B45" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="47"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="44"/>
       <c r="I45" s="33" t="s">
         <v>83</v>
       </c>
@@ -2159,12 +2187,12 @@
       <c r="B46" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="47"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="13"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="44"/>
       <c r="I46" s="33" t="s">
         <v>75</v>
       </c>
@@ -2182,12 +2210,12 @@
       <c r="B47" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="47"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="44"/>
       <c r="I47" s="33" t="s">
         <v>81</v>
       </c>
@@ -2208,12 +2236,12 @@
       <c r="B48" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="47"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="53"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="44"/>
       <c r="I48" s="33" t="s">
         <v>83</v>
       </c>
@@ -2234,12 +2262,12 @@
       <c r="B49" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="47"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="53"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="44"/>
       <c r="I49" s="33" t="s">
         <v>75</v>
       </c>
@@ -2257,12 +2285,12 @@
       <c r="B50" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="47"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="53"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="44"/>
       <c r="I50" s="33" t="s">
         <v>81</v>
       </c>
@@ -2283,12 +2311,12 @@
       <c r="B51" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="47"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="53"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="44"/>
       <c r="I51" s="33" t="s">
         <v>75</v>
       </c>
@@ -2306,12 +2334,12 @@
       <c r="B52" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="47"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="53"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="44"/>
       <c r="I52" s="33" t="s">
         <v>75</v>
       </c>
@@ -2329,12 +2357,12 @@
       <c r="B53" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="47"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="53"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="44"/>
       <c r="I53" s="33" t="s">
         <v>81</v>
       </c>
@@ -2355,12 +2383,12 @@
       <c r="B54" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="47"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="53"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="44"/>
       <c r="I54" s="33" t="s">
         <v>83</v>
       </c>
@@ -2381,12 +2409,12 @@
       <c r="B55" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="47"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="53"/>
       <c r="E55" s="13"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="44"/>
       <c r="I55" s="33" t="s">
         <v>75</v>
       </c>
@@ -2404,12 +2432,12 @@
       <c r="B56" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="44"/>
-      <c r="D56" s="47"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="53"/>
       <c r="E56" s="13"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="44"/>
       <c r="I56" s="33" t="s">
         <v>81</v>
       </c>
@@ -2430,12 +2458,12 @@
       <c r="B57" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="47"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="53"/>
       <c r="E57" s="13"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="44"/>
       <c r="I57" s="33" t="s">
         <v>89</v>
       </c>
@@ -2453,12 +2481,12 @@
       <c r="B58" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="47"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="53"/>
       <c r="E58" s="13"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="44"/>
       <c r="I58" s="33" t="s">
         <v>91</v>
       </c>
@@ -2476,12 +2504,12 @@
       <c r="B59" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="48"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="54"/>
       <c r="E59" s="18"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="45"/>
       <c r="I59" s="34" t="s">
         <v>91</v>
       </c>
@@ -2496,16 +2524,16 @@
       <c r="A60" s="15">
         <v>60</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="35" t="s">
         <v>99</v>
       </c>
       <c r="C60" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="49" t="s">
+      <c r="D60" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="43" t="s">
         <v>101</v>
       </c>
       <c r="F60" s="29" t="s">
@@ -2517,7 +2545,7 @@
       <c r="H60" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I60" s="37" t="s">
+      <c r="I60" s="36" t="s">
         <v>103</v>
       </c>
       <c r="J60" s="30"/>
@@ -2527,14 +2555,14 @@
       <c r="A61" s="15">
         <v>61</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="35" t="s">
         <v>104</v>
       </c>
       <c r="C61" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
       <c r="F61" s="29" t="s">
         <v>102</v>
       </c>
@@ -2544,33 +2572,33 @@
       <c r="H61" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I61" s="37" t="s">
+      <c r="I61" s="36" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" s="55" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>62</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="35" t="s">
+      <c r="F62" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="G62" s="35" t="s">
+      <c r="G62" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H62" s="35" t="s">
+      <c r="H62" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="J62" s="35"/>
+      <c r="J62" s="39"/>
     </row>
     <row r="63" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
@@ -2582,22 +2610,22 @@
       <c r="C63" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="53" t="s">
+      <c r="D63" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E63" s="53">
+      <c r="E63" s="42">
         <v>1</v>
       </c>
-      <c r="F63" s="39" t="s">
+      <c r="F63" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G63" s="38" t="s">
+      <c r="G63" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H63" s="38" t="s">
+      <c r="H63" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I63" s="37" t="s">
+      <c r="I63" s="36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2611,18 +2639,18 @@
       <c r="C64" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="39" t="s">
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G64" s="38" t="s">
+      <c r="G64" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H64" s="38" t="s">
+      <c r="H64" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I64" s="37" t="s">
+      <c r="I64" s="36" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2636,18 +2664,18 @@
       <c r="C65" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="53"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="39" t="s">
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G65" s="38" t="s">
+      <c r="G65" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H65" s="38" t="s">
+      <c r="H65" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I65" s="37" t="s">
+      <c r="I65" s="36" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2661,18 +2689,18 @@
       <c r="C66" t="s">
         <v>105</v>
       </c>
-      <c r="D66" s="53"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="39" t="s">
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G66" s="38" t="s">
+      <c r="G66" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H66" s="38" t="s">
+      <c r="H66" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I66" s="37" t="s">
+      <c r="I66" s="36" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2686,18 +2714,18 @@
       <c r="C67" t="s">
         <v>105</v>
       </c>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="39" t="s">
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G67" s="38" t="s">
+      <c r="G67" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H67" s="38" t="s">
+      <c r="H67" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I67" s="37" t="s">
+      <c r="I67" s="36" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2711,18 +2739,18 @@
       <c r="C68" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="39" t="s">
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="38" t="s">
+      <c r="G68" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H68" s="38" t="s">
+      <c r="H68" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I68" s="37" t="s">
+      <c r="I68" s="36" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2736,18 +2764,18 @@
       <c r="C69" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="39" t="s">
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G69" s="38" t="s">
+      <c r="G69" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H69" s="38" t="s">
+      <c r="H69" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I69" s="37" t="s">
+      <c r="I69" s="36" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2761,18 +2789,18 @@
       <c r="C70" t="s">
         <v>105</v>
       </c>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="39" t="s">
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G70" s="38" t="s">
+      <c r="G70" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H70" s="38" t="s">
+      <c r="H70" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I70" s="52" t="s">
+      <c r="I70" s="41" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2786,41 +2814,49 @@
       <c r="C71" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="53"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="39" t="s">
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="G71" s="38" t="s">
+      <c r="G71" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H71" s="38" t="s">
+      <c r="H71" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I71" s="37" t="s">
+      <c r="I71" s="36" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F72" s="39"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="38"/>
+      <c r="A72" s="15">
+        <v>72</v>
+      </c>
+      <c r="C72" s="57">
+        <v>43210</v>
+      </c>
+      <c r="D72" t="s">
+        <v>122</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G72" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="H72" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="36" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D63:D71"/>
-    <mergeCell ref="E63:E71"/>
-    <mergeCell ref="G2:G16"/>
-    <mergeCell ref="H2:H16"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
-    <mergeCell ref="F19:F34"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="F2:F16"/>
     <mergeCell ref="K19:K34"/>
     <mergeCell ref="F35:F59"/>
     <mergeCell ref="G35:G59"/>
@@ -2831,6 +2867,19 @@
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
     <mergeCell ref="J19:J34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
+    <mergeCell ref="F19:F34"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="F2:F16"/>
+    <mergeCell ref="D63:D71"/>
+    <mergeCell ref="E63:E71"/>
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="H2:H16"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
This Review on the Project plan as it's missing a Change Management Plan and how to handle the change requests.
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.1.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="131">
   <si>
     <t>Review Log</t>
   </si>
@@ -476,11 +476,26 @@
   <si>
     <t>You should put the HLD In a Word file with a a describation  for it</t>
   </si>
+  <si>
+    <t>Omnia/Mona</t>
+  </si>
+  <si>
+    <t>Missing section</t>
+  </si>
+  <si>
+    <t>No Change Management plan to handle any upcoming change request (High risk)</t>
+  </si>
+  <si>
+    <t>invalid as this buttom is connected directly to the power source</t>
+  </si>
+  <si>
+    <t>It was mention as standalone Power source</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,7 +550,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +566,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,13 +845,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -860,13 +881,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
+      <selection pane="bottomLeft" activeCell="J63" sqref="J63:K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,22 +1278,22 @@
       <c r="B2" s="4">
         <v>1.2</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="55">
         <v>2</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="55" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -1265,12 +1309,12 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1284,12 +1328,12 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1303,12 +1347,12 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1322,12 +1366,12 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1341,12 +1385,12 @@
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1360,12 +1404,12 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
       <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1379,12 +1423,12 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1398,12 +1442,12 @@
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1417,12 +1461,12 @@
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="16" t="s">
         <v>28</v>
       </c>
@@ -1436,12 +1480,12 @@
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1455,12 +1499,12 @@
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1474,12 +1518,12 @@
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1493,12 +1537,12 @@
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1512,12 +1556,12 @@
       <c r="B16" s="7">
         <v>2.5</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
       <c r="I16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1593,28 +1637,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="55">
         <v>1</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="55" t="s">
         <v>41</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="55" t="s">
         <v>45</v>
       </c>
       <c r="K19" s="46" t="s">
@@ -1626,16 +1670,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="44"/>
+      <c r="J20" s="56"/>
       <c r="K20" s="47"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1645,16 +1689,16 @@
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="44"/>
+      <c r="J21" s="56"/>
       <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1664,16 +1708,16 @@
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="44"/>
+      <c r="J22" s="56"/>
       <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1683,16 +1727,16 @@
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="44"/>
+      <c r="J23" s="56"/>
       <c r="K23" s="47"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,16 +1746,16 @@
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="44"/>
+      <c r="J24" s="56"/>
       <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1721,16 +1765,16 @@
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="44"/>
+      <c r="J25" s="56"/>
       <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1740,16 +1784,16 @@
       <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="44"/>
+      <c r="J26" s="56"/>
       <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1757,16 +1801,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="44"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="47"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1776,16 +1820,16 @@
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="44"/>
+      <c r="J28" s="56"/>
       <c r="K28" s="47"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1795,16 +1839,16 @@
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="44"/>
+      <c r="J29" s="56"/>
       <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1814,16 +1858,16 @@
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="44"/>
+      <c r="J30" s="56"/>
       <c r="K30" s="47"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1833,16 +1877,16 @@
       <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="44"/>
+      <c r="J31" s="56"/>
       <c r="K31" s="47"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,16 +1896,16 @@
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
       <c r="I32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="44"/>
+      <c r="J32" s="56"/>
       <c r="K32" s="47"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1871,16 +1915,16 @@
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
       <c r="I33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J33" s="44"/>
+      <c r="J33" s="56"/>
       <c r="K33" s="47"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1890,16 +1934,16 @@
       <c r="B34" s="7">
         <v>6.2</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
       <c r="I34" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="45"/>
+      <c r="J34" s="57"/>
       <c r="K34" s="48"/>
     </row>
     <row r="35" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1922,7 +1966,7 @@
       <c r="G35" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="43" t="s">
+      <c r="H35" s="55" t="s">
         <v>73</v>
       </c>
       <c r="I35" s="32" t="s">
@@ -1947,7 +1991,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="50"/>
       <c r="G36" s="50"/>
-      <c r="H36" s="44"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="33" t="s">
         <v>75</v>
       </c>
@@ -1970,7 +2014,7 @@
       <c r="E37" s="13"/>
       <c r="F37" s="50"/>
       <c r="G37" s="50"/>
-      <c r="H37" s="44"/>
+      <c r="H37" s="56"/>
       <c r="I37" s="33" t="s">
         <v>76</v>
       </c>
@@ -1996,7 +2040,7 @@
       <c r="E38" s="13"/>
       <c r="F38" s="50"/>
       <c r="G38" s="50"/>
-      <c r="H38" s="44"/>
+      <c r="H38" s="56"/>
       <c r="I38" s="33" t="s">
         <v>78</v>
       </c>
@@ -2019,7 +2063,7 @@
       <c r="E39" s="13"/>
       <c r="F39" s="50"/>
       <c r="G39" s="50"/>
-      <c r="H39" s="44"/>
+      <c r="H39" s="56"/>
       <c r="I39" s="33" t="s">
         <v>75</v>
       </c>
@@ -2042,7 +2086,7 @@
       <c r="E40" s="13"/>
       <c r="F40" s="50"/>
       <c r="G40" s="50"/>
-      <c r="H40" s="44"/>
+      <c r="H40" s="56"/>
       <c r="I40" s="33" t="s">
         <v>76</v>
       </c>
@@ -2068,7 +2112,7 @@
       <c r="E41" s="13"/>
       <c r="F41" s="50"/>
       <c r="G41" s="50"/>
-      <c r="H41" s="44"/>
+      <c r="H41" s="56"/>
       <c r="I41" s="33" t="s">
         <v>75</v>
       </c>
@@ -2091,7 +2135,7 @@
       <c r="E42" s="13"/>
       <c r="F42" s="50"/>
       <c r="G42" s="50"/>
-      <c r="H42" s="44"/>
+      <c r="H42" s="56"/>
       <c r="I42" s="33" t="s">
         <v>76</v>
       </c>
@@ -2117,7 +2161,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="50"/>
       <c r="G43" s="50"/>
-      <c r="H43" s="44"/>
+      <c r="H43" s="56"/>
       <c r="I43" s="33" t="s">
         <v>75</v>
       </c>
@@ -2140,7 +2184,7 @@
       <c r="E44" s="13"/>
       <c r="F44" s="50"/>
       <c r="G44" s="50"/>
-      <c r="H44" s="44"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="33" t="s">
         <v>81</v>
       </c>
@@ -2166,7 +2210,7 @@
       <c r="E45" s="13"/>
       <c r="F45" s="50"/>
       <c r="G45" s="50"/>
-      <c r="H45" s="44"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="33" t="s">
         <v>83</v>
       </c>
@@ -2192,7 +2236,7 @@
       <c r="E46" s="13"/>
       <c r="F46" s="50"/>
       <c r="G46" s="50"/>
-      <c r="H46" s="44"/>
+      <c r="H46" s="56"/>
       <c r="I46" s="33" t="s">
         <v>75</v>
       </c>
@@ -2215,7 +2259,7 @@
       <c r="E47" s="13"/>
       <c r="F47" s="50"/>
       <c r="G47" s="50"/>
-      <c r="H47" s="44"/>
+      <c r="H47" s="56"/>
       <c r="I47" s="33" t="s">
         <v>81</v>
       </c>
@@ -2241,7 +2285,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="50"/>
       <c r="G48" s="50"/>
-      <c r="H48" s="44"/>
+      <c r="H48" s="56"/>
       <c r="I48" s="33" t="s">
         <v>83</v>
       </c>
@@ -2267,7 +2311,7 @@
       <c r="E49" s="13"/>
       <c r="F49" s="50"/>
       <c r="G49" s="50"/>
-      <c r="H49" s="44"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="33" t="s">
         <v>75</v>
       </c>
@@ -2290,7 +2334,7 @@
       <c r="E50" s="13"/>
       <c r="F50" s="50"/>
       <c r="G50" s="50"/>
-      <c r="H50" s="44"/>
+      <c r="H50" s="56"/>
       <c r="I50" s="33" t="s">
         <v>81</v>
       </c>
@@ -2316,7 +2360,7 @@
       <c r="E51" s="13"/>
       <c r="F51" s="50"/>
       <c r="G51" s="50"/>
-      <c r="H51" s="44"/>
+      <c r="H51" s="56"/>
       <c r="I51" s="33" t="s">
         <v>75</v>
       </c>
@@ -2339,7 +2383,7 @@
       <c r="E52" s="13"/>
       <c r="F52" s="50"/>
       <c r="G52" s="50"/>
-      <c r="H52" s="44"/>
+      <c r="H52" s="56"/>
       <c r="I52" s="33" t="s">
         <v>75</v>
       </c>
@@ -2362,7 +2406,7 @@
       <c r="E53" s="13"/>
       <c r="F53" s="50"/>
       <c r="G53" s="50"/>
-      <c r="H53" s="44"/>
+      <c r="H53" s="56"/>
       <c r="I53" s="33" t="s">
         <v>81</v>
       </c>
@@ -2388,7 +2432,7 @@
       <c r="E54" s="13"/>
       <c r="F54" s="50"/>
       <c r="G54" s="50"/>
-      <c r="H54" s="44"/>
+      <c r="H54" s="56"/>
       <c r="I54" s="33" t="s">
         <v>83</v>
       </c>
@@ -2414,7 +2458,7 @@
       <c r="E55" s="13"/>
       <c r="F55" s="50"/>
       <c r="G55" s="50"/>
-      <c r="H55" s="44"/>
+      <c r="H55" s="56"/>
       <c r="I55" s="33" t="s">
         <v>75</v>
       </c>
@@ -2437,7 +2481,7 @@
       <c r="E56" s="13"/>
       <c r="F56" s="50"/>
       <c r="G56" s="50"/>
-      <c r="H56" s="44"/>
+      <c r="H56" s="56"/>
       <c r="I56" s="33" t="s">
         <v>81</v>
       </c>
@@ -2463,7 +2507,7 @@
       <c r="E57" s="13"/>
       <c r="F57" s="50"/>
       <c r="G57" s="50"/>
-      <c r="H57" s="44"/>
+      <c r="H57" s="56"/>
       <c r="I57" s="33" t="s">
         <v>89</v>
       </c>
@@ -2486,7 +2530,7 @@
       <c r="E58" s="13"/>
       <c r="F58" s="50"/>
       <c r="G58" s="50"/>
-      <c r="H58" s="44"/>
+      <c r="H58" s="56"/>
       <c r="I58" s="33" t="s">
         <v>91</v>
       </c>
@@ -2509,7 +2553,7 @@
       <c r="E59" s="18"/>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
-      <c r="H59" s="45"/>
+      <c r="H59" s="57"/>
       <c r="I59" s="34" t="s">
         <v>91</v>
       </c>
@@ -2530,10 +2574,10 @@
       <c r="C60" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="43" t="s">
+      <c r="D60" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E60" s="55" t="s">
         <v>101</v>
       </c>
       <c r="F60" s="29" t="s">
@@ -2561,8 +2605,8 @@
       <c r="C61" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56"/>
       <c r="F61" s="29" t="s">
         <v>102</v>
       </c>
@@ -2576,17 +2620,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="55" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" s="44" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>62</v>
       </c>
-      <c r="C62" s="55" t="s">
+      <c r="C62" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="D62" s="55" t="s">
+      <c r="D62" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="44" t="s">
         <v>107</v>
       </c>
       <c r="F62" s="39" t="s">
@@ -2595,7 +2639,7 @@
       <c r="G62" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H62" s="56" t="s">
+      <c r="H62" s="45" t="s">
         <v>110</v>
       </c>
       <c r="J62" s="39"/>
@@ -2610,10 +2654,10 @@
       <c r="C63" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="E63" s="42">
+      <c r="E63" s="58">
         <v>1</v>
       </c>
       <c r="F63" s="38" t="s">
@@ -2627,6 +2671,12 @@
       </c>
       <c r="I63" s="36" t="s">
         <v>113</v>
+      </c>
+      <c r="J63" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K63" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2639,8 +2689,8 @@
       <c r="C64" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
       <c r="F64" s="38" t="s">
         <v>112</v>
       </c>
@@ -2653,8 +2703,14 @@
       <c r="I64" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J64" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>65</v>
       </c>
@@ -2664,8 +2720,8 @@
       <c r="C65" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
       <c r="F65" s="38" t="s">
         <v>112</v>
       </c>
@@ -2678,8 +2734,14 @@
       <c r="I65" s="36" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="K65" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>66</v>
       </c>
@@ -2689,8 +2751,8 @@
       <c r="C66" t="s">
         <v>105</v>
       </c>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="58"/>
       <c r="F66" s="38" t="s">
         <v>112</v>
       </c>
@@ -2703,8 +2765,14 @@
       <c r="I66" s="36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J66" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>67</v>
       </c>
@@ -2714,8 +2782,8 @@
       <c r="C67" t="s">
         <v>105</v>
       </c>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="58"/>
       <c r="F67" s="38" t="s">
         <v>112</v>
       </c>
@@ -2728,8 +2796,14 @@
       <c r="I67" s="36" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J67" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>68</v>
       </c>
@@ -2739,8 +2813,8 @@
       <c r="C68" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
+      <c r="D68" s="58"/>
+      <c r="E68" s="58"/>
       <c r="F68" s="38" t="s">
         <v>112</v>
       </c>
@@ -2753,8 +2827,14 @@
       <c r="I68" s="36" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J68" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>69</v>
       </c>
@@ -2764,8 +2844,8 @@
       <c r="C69" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="42"/>
-      <c r="E69" s="42"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
       <c r="F69" s="38" t="s">
         <v>112</v>
       </c>
@@ -2778,8 +2858,14 @@
       <c r="I69" s="36" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J69" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K69" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>70</v>
       </c>
@@ -2789,8 +2875,8 @@
       <c r="C70" t="s">
         <v>105</v>
       </c>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
       <c r="F70" s="38" t="s">
         <v>112</v>
       </c>
@@ -2803,8 +2889,14 @@
       <c r="I70" s="41" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J70" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="K70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>71</v>
       </c>
@@ -2814,8 +2906,8 @@
       <c r="C71" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="42"/>
-      <c r="E71" s="42"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="58"/>
       <c r="F71" s="38" t="s">
         <v>112</v>
       </c>
@@ -2828,18 +2920,24 @@
       <c r="I71" s="36" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K71" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <v>72</v>
       </c>
-      <c r="C72" s="57">
-        <v>43210</v>
+      <c r="C72" t="s">
+        <v>105</v>
       </c>
       <c r="D72" t="s">
         <v>122</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="42">
         <v>1</v>
       </c>
       <c r="F72" s="38" t="s">
@@ -2855,8 +2953,48 @@
         <v>125</v>
       </c>
     </row>
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
+        <v>73</v>
+      </c>
+      <c r="B73" s="59"/>
+      <c r="C73" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="63">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F73" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="G73" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H73" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="I73" s="62" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D63:D71"/>
+    <mergeCell ref="E63:E71"/>
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="H2:H16"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
+    <mergeCell ref="F19:F34"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="F2:F16"/>
     <mergeCell ref="K19:K34"/>
     <mergeCell ref="F35:F59"/>
     <mergeCell ref="G35:G59"/>
@@ -2867,19 +3005,6 @@
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
     <mergeCell ref="J19:J34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
-    <mergeCell ref="F19:F34"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="F2:F16"/>
-    <mergeCell ref="D63:D71"/>
-    <mergeCell ref="E63:E71"/>
-    <mergeCell ref="G2:G16"/>
-    <mergeCell ref="H2:H16"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Upload Reviewing on CDD of ICU
Upload Reviewing on CDD of ICU
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.1.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="135">
   <si>
     <t>Review Log</t>
   </si>
@@ -90,13 +90,7 @@
     <t xml:space="preserve">2.2.7 </t>
   </si>
   <si>
-    <t xml:space="preserve">determination the scale  time ,scale speed   </t>
-  </si>
-  <si>
     <t>2.2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">please refer  the number of function caver this point </t>
   </si>
   <si>
     <t xml:space="preserve">2.2.9 </t>
@@ -477,19 +471,37 @@
     <t>You should put the HLD In a Word file with a a describation  for it</t>
   </si>
   <si>
-    <t>Omnia/Mona</t>
-  </si>
-  <si>
-    <t>Missing section</t>
-  </si>
-  <si>
-    <t>No Change Management plan to handle any upcoming change request (High risk)</t>
-  </si>
-  <si>
-    <t>invalid as this buttom is connected directly to the power source</t>
-  </si>
-  <si>
-    <t>It was mention as standalone Power source</t>
+    <t>already mentioned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding required info.   </t>
+  </si>
+  <si>
+    <t>adding required info.</t>
+  </si>
+  <si>
+    <t>any barrier of any kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">done </t>
+  </si>
+  <si>
+    <t>not assigned for me</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Component_Design_Document_ICU</t>
+  </si>
+  <si>
+    <t>Ahmed Eldakak</t>
+  </si>
+  <si>
+    <t>Yasmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to change header </t>
   </si>
 </sst>
 </file>
@@ -550,7 +562,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,12 +578,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -842,9 +848,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,6 +857,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -893,24 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,7 +958,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1006,7 +993,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1215,11 +1202,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J63" sqref="J63:K71"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="A74:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,16 +1228,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
@@ -1279,7 +1266,7 @@
         <v>1.2</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>9</v>
@@ -1294,12 +1281,14 @@
         <v>11</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1318,7 +1307,9 @@
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1337,7 +1328,9 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1356,7 +1349,9 @@
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="59" t="s">
+        <v>126</v>
+      </c>
       <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1375,7 +1370,9 @@
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="J6" s="59" t="s">
+        <v>126</v>
+      </c>
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,7 +1391,9 @@
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1413,10 +1412,12 @@
       <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="59" t="s">
+        <v>126</v>
+      </c>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1429,8 +1430,8 @@
       <c r="F9" s="56"/>
       <c r="G9" s="56"/>
       <c r="H9" s="56"/>
-      <c r="I9" s="2" t="s">
-        <v>24</v>
+      <c r="I9" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
@@ -1440,7 +1441,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
@@ -1449,17 +1450,19 @@
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
       <c r="I10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>126</v>
+      </c>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
@@ -1467,10 +1470,12 @@
       <c r="F11" s="56"/>
       <c r="G11" s="56"/>
       <c r="H11" s="56"/>
-      <c r="I11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="13"/>
+      <c r="I11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="56"/>
       <c r="D12" s="56"/>
@@ -1487,9 +1492,11 @@
       <c r="G12" s="56"/>
       <c r="H12" s="56"/>
       <c r="I12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="J12" s="59" t="s">
+        <v>127</v>
+      </c>
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1497,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
@@ -1506,17 +1513,19 @@
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="56"/>
@@ -1524,18 +1533,20 @@
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
       <c r="H14" s="56"/>
-      <c r="I14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="13"/>
+      <c r="I14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="59" t="s">
+        <v>128</v>
+      </c>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
@@ -1543,13 +1554,15 @@
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
-      <c r="I15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="13"/>
+      <c r="I15" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="59" t="s">
+        <v>129</v>
+      </c>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -1562,19 +1575,21 @@
       <c r="F16" s="57"/>
       <c r="G16" s="57"/>
       <c r="H16" s="57"/>
-      <c r="I16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="18"/>
+      <c r="I16" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>129</v>
+      </c>
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>15</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>0</v>
@@ -1583,53 +1598,53 @@
         <v>2</v>
       </c>
       <c r="F17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>42</v>
+      <c r="I17" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>16</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>44</v>
+      <c r="I18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1638,31 +1653,31 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" s="55">
         <v>1</v>
       </c>
       <c r="F19" s="55" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G19" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K19" s="46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1782,7 +1797,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="56"/>
@@ -1875,7 +1890,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C31" s="56"/>
       <c r="D31" s="56"/>
@@ -1889,7 +1904,7 @@
       <c r="J31" s="56"/>
       <c r="K31" s="47"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>32</v>
       </c>
@@ -1902,13 +1917,13 @@
       <c r="F32" s="56"/>
       <c r="G32" s="56"/>
       <c r="H32" s="56"/>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="7" t="s">
         <v>64</v>
       </c>
       <c r="J32" s="56"/>
       <c r="K32" s="47"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>33</v>
       </c>
@@ -1921,13 +1936,13 @@
       <c r="F33" s="56"/>
       <c r="G33" s="56"/>
       <c r="H33" s="56"/>
-      <c r="I33" s="2" t="s">
-        <v>65</v>
+      <c r="I33" s="32" t="s">
+        <v>72</v>
       </c>
       <c r="J33" s="56"/>
       <c r="K33" s="47"/>
     </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>34</v>
       </c>
@@ -1940,51 +1955,51 @@
       <c r="F34" s="57"/>
       <c r="G34" s="57"/>
       <c r="H34" s="57"/>
-      <c r="I34" s="7" t="s">
-        <v>66</v>
+      <c r="I34" s="33" t="s">
+        <v>73</v>
       </c>
       <c r="J34" s="57"/>
       <c r="K34" s="48"/>
     </row>
-    <row r="35" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31">
         <v>35</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G35" s="49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" s="33" t="s">
         <v>74</v>
       </c>
       <c r="J35" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K35" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>36</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="50"/>
       <c r="D36" s="53"/>
@@ -1993,21 +2008,21 @@
       <c r="G36" s="50"/>
       <c r="H36" s="56"/>
       <c r="I36" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K36" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="50"/>
       <c r="D37" s="53"/>
@@ -2016,16 +2031,16 @@
       <c r="G37" s="50"/>
       <c r="H37" s="56"/>
       <c r="I37" s="33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J37" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2048,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="50"/>
       <c r="D38" s="53"/>
@@ -2042,13 +2057,13 @@
       <c r="G38" s="50"/>
       <c r="H38" s="56"/>
       <c r="I38" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J38" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2056,7 +2071,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="50"/>
       <c r="D39" s="53"/>
@@ -2065,13 +2080,13 @@
       <c r="G39" s="50"/>
       <c r="H39" s="56"/>
       <c r="I39" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K39" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2079,7 +2094,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="50"/>
       <c r="D40" s="53"/>
@@ -2088,16 +2103,16 @@
       <c r="G40" s="50"/>
       <c r="H40" s="56"/>
       <c r="I40" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J40" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K40" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2105,7 +2120,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="50"/>
       <c r="D41" s="53"/>
@@ -2114,21 +2129,21 @@
       <c r="G41" s="50"/>
       <c r="H41" s="56"/>
       <c r="I41" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J41" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K41" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>42</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" s="50"/>
       <c r="D42" s="53"/>
@@ -2137,24 +2152,24 @@
       <c r="G42" s="50"/>
       <c r="H42" s="56"/>
       <c r="I42" s="33" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J42" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>43</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="50"/>
       <c r="D43" s="53"/>
@@ -2163,13 +2178,13 @@
       <c r="G43" s="50"/>
       <c r="H43" s="56"/>
       <c r="I43" s="33" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J43" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K43" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2192,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C44" s="50"/>
       <c r="D44" s="53"/>
@@ -2186,24 +2201,24 @@
       <c r="G44" s="50"/>
       <c r="H44" s="56"/>
       <c r="I44" s="33" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K44" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>45</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C45" s="50"/>
       <c r="D45" s="53"/>
@@ -2212,24 +2227,24 @@
       <c r="G45" s="50"/>
       <c r="H45" s="56"/>
       <c r="I45" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K45" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="L45" t="s">
         <v>94</v>
       </c>
-      <c r="L45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>46</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="50"/>
       <c r="D46" s="53"/>
@@ -2238,13 +2253,13 @@
       <c r="G46" s="50"/>
       <c r="H46" s="56"/>
       <c r="I46" s="33" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K46" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2252,7 +2267,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C47" s="50"/>
       <c r="D47" s="53"/>
@@ -2261,24 +2276,24 @@
       <c r="G47" s="50"/>
       <c r="H47" s="56"/>
       <c r="I47" s="33" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J47" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K47" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>48</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C48" s="50"/>
       <c r="D48" s="53"/>
@@ -2287,16 +2302,16 @@
       <c r="G48" s="50"/>
       <c r="H48" s="56"/>
       <c r="I48" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K48" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" t="s">
         <v>94</v>
-      </c>
-      <c r="L48" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2304,7 +2319,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" s="50"/>
       <c r="D49" s="53"/>
@@ -2313,13 +2328,13 @@
       <c r="G49" s="50"/>
       <c r="H49" s="56"/>
       <c r="I49" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J49" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K49" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2327,7 +2342,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C50" s="50"/>
       <c r="D50" s="53"/>
@@ -2336,16 +2351,16 @@
       <c r="G50" s="50"/>
       <c r="H50" s="56"/>
       <c r="I50" s="33" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J50" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K50" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2353,7 +2368,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" s="50"/>
       <c r="D51" s="53"/>
@@ -2362,21 +2377,21 @@
       <c r="G51" s="50"/>
       <c r="H51" s="56"/>
       <c r="I51" s="33" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K51" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>52</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C52" s="50"/>
       <c r="D52" s="53"/>
@@ -2385,13 +2400,13 @@
       <c r="G52" s="50"/>
       <c r="H52" s="56"/>
       <c r="I52" s="33" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J52" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K52" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2399,7 +2414,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="53"/>
@@ -2408,24 +2423,24 @@
       <c r="G53" s="50"/>
       <c r="H53" s="56"/>
       <c r="I53" s="33" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J53" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K53" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L53" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>54</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" s="50"/>
       <c r="D54" s="53"/>
@@ -2434,24 +2449,24 @@
       <c r="G54" s="50"/>
       <c r="H54" s="56"/>
       <c r="I54" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J54" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K54" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="L54" t="s">
         <v>94</v>
       </c>
-      <c r="L54" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>55</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C55" s="50"/>
       <c r="D55" s="53"/>
@@ -2460,21 +2475,21 @@
       <c r="G55" s="50"/>
       <c r="H55" s="56"/>
       <c r="I55" s="33" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="J55" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K55" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>56</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C56" s="50"/>
       <c r="D56" s="53"/>
@@ -2483,16 +2498,16 @@
       <c r="G56" s="50"/>
       <c r="H56" s="56"/>
       <c r="I56" s="33" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J56" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K56" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2500,7 +2515,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C57" s="50"/>
       <c r="D57" s="53"/>
@@ -2508,14 +2523,14 @@
       <c r="F57" s="50"/>
       <c r="G57" s="50"/>
       <c r="H57" s="56"/>
-      <c r="I57" s="33" t="s">
+      <c r="I57" s="34" t="s">
         <v>89</v>
       </c>
       <c r="J57" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K57" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2523,7 +2538,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C58" s="50"/>
       <c r="D58" s="53"/>
@@ -2531,14 +2546,14 @@
       <c r="F58" s="50"/>
       <c r="G58" s="50"/>
       <c r="H58" s="56"/>
-      <c r="I58" s="33" t="s">
-        <v>91</v>
+      <c r="I58" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="J58" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K58" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2546,7 +2561,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C59" s="51"/>
       <c r="D59" s="54"/>
@@ -2554,45 +2569,45 @@
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
       <c r="H59" s="57"/>
-      <c r="I59" s="34" t="s">
-        <v>91</v>
+      <c r="I59" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="J59" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>60</v>
       </c>
       <c r="B60" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="E60" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C60" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="55" t="s">
+      <c r="F60" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E60" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="F60" s="29" t="s">
-        <v>102</v>
-      </c>
       <c r="G60" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H60" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="I60" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="J60" s="30"/>
+        <v>70</v>
+      </c>
+      <c r="H60" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="I60" s="43"/>
+      <c r="J60" s="30" t="s">
+        <v>130</v>
+      </c>
       <c r="K60" s="30"/>
     </row>
     <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2600,51 +2615,57 @@
         <v>61</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D61" s="56"/>
       <c r="E61" s="56"/>
       <c r="F61" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H61" s="29" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="H61" s="44" t="s">
+        <v>108</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="44" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="J61" s="42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="43" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>62</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="D62" s="44" t="s">
+      <c r="F62" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="E62" s="44" t="s">
+      <c r="G62" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="39" t="s">
+      <c r="H62" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="G62" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="H62" s="45" t="s">
-        <v>110</v>
+      <c r="I62" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="J62" s="39"/>
     </row>
-    <row r="63" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>63</v>
       </c>
@@ -2652,31 +2673,25 @@
         <v>1.4</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D63" s="58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E63" s="58">
         <v>1</v>
       </c>
       <c r="F63" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G63" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H63" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I63" s="36" t="s">
         <v>113</v>
-      </c>
-      <c r="J63" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K63" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2687,30 +2702,24 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D64" s="58"/>
       <c r="E64" s="58"/>
       <c r="F64" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G64" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H64" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I64" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="J64" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K64" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>65</v>
       </c>
@@ -2718,30 +2727,24 @@
         <v>2.1</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D65" s="58"/>
       <c r="E65" s="58"/>
       <c r="F65" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G65" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H65" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I65" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="J65" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="K65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>66</v>
       </c>
@@ -2749,30 +2752,24 @@
         <v>7.2</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D66" s="58"/>
       <c r="E66" s="58"/>
       <c r="F66" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G66" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H66" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I66" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="J66" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>67</v>
       </c>
@@ -2780,30 +2777,24 @@
         <v>7.2</v>
       </c>
       <c r="C67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D67" s="58"/>
       <c r="E67" s="58"/>
       <c r="F67" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G67" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H67" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I67" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="J67" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>68</v>
       </c>
@@ -2811,30 +2802,24 @@
         <v>7.2</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D68" s="58"/>
       <c r="E68" s="58"/>
       <c r="F68" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G68" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H68" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I68" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="J68" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K68" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="I68" s="41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>69</v>
       </c>
@@ -2842,30 +2827,24 @@
         <v>7.4</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D69" s="58"/>
       <c r="E69" s="58"/>
       <c r="F69" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G69" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H69" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I69" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="J69" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K69" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>70</v>
       </c>
@@ -2873,30 +2852,24 @@
         <v>8.1</v>
       </c>
       <c r="C70" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D70" s="58"/>
       <c r="E70" s="58"/>
       <c r="F70" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G70" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H70" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="J70" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="K70" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="I70" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>71</v>
       </c>
@@ -2904,81 +2877,74 @@
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D71" s="58"/>
       <c r="E71" s="58"/>
       <c r="F71" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G71" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H71" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I71" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="J71" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K71" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>72</v>
       </c>
-      <c r="C72" t="s">
-        <v>105</v>
+      <c r="C72" s="45">
+        <v>43210</v>
       </c>
       <c r="D72" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="G72" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="E72" s="42">
-        <v>1</v>
-      </c>
-      <c r="F72" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="G72" s="37" t="s">
-        <v>124</v>
-      </c>
       <c r="H72" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="I72" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>73</v>
       </c>
-      <c r="B73" s="59"/>
-      <c r="C73" s="64" t="s">
+      <c r="C73" s="45">
+        <v>43210</v>
+      </c>
+      <c r="D73" t="s">
+        <v>131</v>
+      </c>
+      <c r="E73" t="s">
         <v>105</v>
       </c>
-      <c r="D73" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="63">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F73" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="G73" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H73" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="I73" s="62" t="s">
-        <v>128</v>
-      </c>
+      <c r="F73" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="G73" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H73" t="s">
+        <v>39</v>
+      </c>
+      <c r="I73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="C74" s="45"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
review on CDD_os , owner : mustafa
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.1.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="137">
   <si>
     <t>Review Log</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t xml:space="preserve">need to change header </t>
+  </si>
+  <si>
+    <t>moustafa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to change title </t>
   </si>
 </sst>
 </file>
@@ -737,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -858,6 +864,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,19 +907,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,9 +1213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="A74:I74"/>
+      <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,29 +1267,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>1.2</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="49">
         <v>2</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="49" t="s">
         <v>108</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -1298,12 +1307,12 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1319,12 +1328,12 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1340,16 +1349,16 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="47" t="s">
         <v>126</v>
       </c>
       <c r="K5" s="14"/>
@@ -1361,16 +1370,16 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="J6" s="47" t="s">
         <v>126</v>
       </c>
       <c r="K6" s="14"/>
@@ -1382,12 +1391,12 @@
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1396,23 +1405,23 @@
       </c>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
       <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="47" t="s">
         <v>126</v>
       </c>
       <c r="K8" s="14"/>
@@ -1424,12 +1433,12 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="16" t="s">
         <v>26</v>
       </c>
@@ -1443,16 +1452,16 @@
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
       <c r="I10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="47" t="s">
         <v>126</v>
       </c>
       <c r="K10" s="14"/>
@@ -1464,12 +1473,12 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1485,16 +1494,16 @@
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="47" t="s">
         <v>127</v>
       </c>
       <c r="K12" s="14"/>
@@ -1506,12 +1515,12 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1527,16 +1536,16 @@
       <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="47" t="s">
         <v>128</v>
       </c>
       <c r="K14" s="14"/>
@@ -1548,16 +1557,16 @@
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="J15" s="47" t="s">
         <v>129</v>
       </c>
       <c r="K15" s="14"/>
@@ -1569,12 +1578,12 @@
       <c r="B16" s="7">
         <v>2.5</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="24" t="s">
         <v>42</v>
       </c>
@@ -1652,31 +1661,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="55">
+      <c r="E19" s="49">
         <v>1</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="55" t="s">
+      <c r="G19" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="49" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="55" t="s">
+      <c r="J19" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="52" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1685,17 +1694,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="56"/>
-      <c r="K20" s="47"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -1704,17 +1713,17 @@
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="47"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="53"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -1723,17 +1732,17 @@
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="56"/>
-      <c r="K22" s="47"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="53"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -1742,17 +1751,17 @@
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="56"/>
-      <c r="K23" s="47"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="53"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1761,17 +1770,17 @@
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="56"/>
-      <c r="K24" s="47"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="53"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1780,17 +1789,17 @@
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="56"/>
-      <c r="K25" s="47"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="53"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1799,34 +1808,34 @@
       <c r="B26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="56"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="53"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="56"/>
-      <c r="K27" s="47"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="53"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1835,17 +1844,17 @@
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="56"/>
-      <c r="K28" s="47"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="53"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1854,17 +1863,17 @@
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="56"/>
-      <c r="K29" s="47"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="53"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1873,17 +1882,17 @@
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="56"/>
-      <c r="K30" s="47"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -1892,17 +1901,17 @@
       <c r="B31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="47"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="53"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -1911,17 +1920,17 @@
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
       <c r="I32" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="56"/>
-      <c r="K32" s="47"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="53"/>
     </row>
     <row r="33" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1930,17 +1939,17 @@
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
       <c r="I33" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="J33" s="56"/>
-      <c r="K33" s="47"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="53"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
@@ -1949,17 +1958,17 @@
       <c r="B34" s="7">
         <v>6.2</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="57"/>
-      <c r="K34" s="48"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="54"/>
     </row>
     <row r="35" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31">
@@ -1968,20 +1977,20 @@
       <c r="B35" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="58" t="s">
         <v>69</v>
       </c>
       <c r="E35" s="11"/>
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="49" t="s">
+      <c r="G35" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="55" t="s">
+      <c r="H35" s="49" t="s">
         <v>71</v>
       </c>
       <c r="I35" s="33" t="s">
@@ -2001,12 +2010,12 @@
       <c r="B36" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="53"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="50"/>
       <c r="I36" s="33" t="s">
         <v>76</v>
       </c>
@@ -2024,12 +2033,12 @@
       <c r="B37" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="53"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="59"/>
       <c r="E37" s="13"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="50"/>
       <c r="I37" s="33" t="s">
         <v>73</v>
       </c>
@@ -2050,12 +2059,12 @@
       <c r="B38" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="53"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="59"/>
       <c r="E38" s="13"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="33" t="s">
         <v>74</v>
       </c>
@@ -2073,12 +2082,12 @@
       <c r="B39" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="53"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="59"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="50"/>
       <c r="I39" s="33" t="s">
         <v>73</v>
       </c>
@@ -2096,12 +2105,12 @@
       <c r="B40" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="53"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="59"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="50"/>
       <c r="I40" s="33" t="s">
         <v>74</v>
       </c>
@@ -2122,12 +2131,12 @@
       <c r="B41" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="53"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="59"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="50"/>
       <c r="I41" s="33" t="s">
         <v>73</v>
       </c>
@@ -2145,12 +2154,12 @@
       <c r="B42" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="53"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="59"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="33" t="s">
         <v>79</v>
       </c>
@@ -2171,12 +2180,12 @@
       <c r="B43" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="53"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="59"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="56"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="50"/>
       <c r="I43" s="33" t="s">
         <v>81</v>
       </c>
@@ -2194,12 +2203,12 @@
       <c r="B44" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="50"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="50"/>
       <c r="I44" s="33" t="s">
         <v>73</v>
       </c>
@@ -2220,12 +2229,12 @@
       <c r="B45" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="53"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="50"/>
       <c r="I45" s="33" t="s">
         <v>79</v>
       </c>
@@ -2246,12 +2255,12 @@
       <c r="B46" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="50"/>
-      <c r="D46" s="53"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="59"/>
       <c r="E46" s="13"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="50"/>
       <c r="I46" s="33" t="s">
         <v>81</v>
       </c>
@@ -2269,12 +2278,12 @@
       <c r="B47" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="53"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="50"/>
       <c r="I47" s="33" t="s">
         <v>73</v>
       </c>
@@ -2295,12 +2304,12 @@
       <c r="B48" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="53"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="59"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="50"/>
       <c r="I48" s="33" t="s">
         <v>79</v>
       </c>
@@ -2321,12 +2330,12 @@
       <c r="B49" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="53"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="59"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="50"/>
       <c r="I49" s="33" t="s">
         <v>73</v>
       </c>
@@ -2344,12 +2353,12 @@
       <c r="B50" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="53"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="59"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="50"/>
       <c r="I50" s="33" t="s">
         <v>73</v>
       </c>
@@ -2370,12 +2379,12 @@
       <c r="B51" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="50"/>
-      <c r="D51" s="53"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="59"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="50"/>
       <c r="I51" s="33" t="s">
         <v>79</v>
       </c>
@@ -2393,12 +2402,12 @@
       <c r="B52" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="50"/>
-      <c r="D52" s="53"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="59"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="50"/>
       <c r="I52" s="33" t="s">
         <v>81</v>
       </c>
@@ -2416,12 +2425,12 @@
       <c r="B53" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="50"/>
-      <c r="D53" s="53"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="59"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="50"/>
       <c r="I53" s="33" t="s">
         <v>73</v>
       </c>
@@ -2442,12 +2451,12 @@
       <c r="B54" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="50"/>
-      <c r="D54" s="53"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="59"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="50"/>
       <c r="I54" s="33" t="s">
         <v>79</v>
       </c>
@@ -2468,12 +2477,12 @@
       <c r="B55" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="50"/>
-      <c r="D55" s="53"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="59"/>
       <c r="E55" s="13"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="50"/>
       <c r="I55" s="33" t="s">
         <v>87</v>
       </c>
@@ -2491,12 +2500,12 @@
       <c r="B56" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="50"/>
-      <c r="D56" s="53"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="59"/>
       <c r="E56" s="13"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="50"/>
       <c r="I56" s="33" t="s">
         <v>89</v>
       </c>
@@ -2517,12 +2526,12 @@
       <c r="B57" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="50"/>
-      <c r="D57" s="53"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="59"/>
       <c r="E57" s="13"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="50"/>
       <c r="I57" s="34" t="s">
         <v>89</v>
       </c>
@@ -2540,12 +2549,12 @@
       <c r="B58" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="50"/>
-      <c r="D58" s="53"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="59"/>
       <c r="E58" s="13"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="50"/>
       <c r="I58" s="36" t="s">
         <v>101</v>
       </c>
@@ -2563,12 +2572,12 @@
       <c r="B59" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="51"/>
-      <c r="D59" s="54"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="60"/>
       <c r="E59" s="18"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="51"/>
       <c r="I59" s="36" t="s">
         <v>101</v>
       </c>
@@ -2589,10 +2598,10 @@
       <c r="C60" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="55" t="s">
+      <c r="D60" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E60" s="55" t="s">
+      <c r="E60" s="49" t="s">
         <v>99</v>
       </c>
       <c r="F60" s="29" t="s">
@@ -2620,8 +2629,8 @@
       <c r="C61" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
       <c r="F61" s="29" t="s">
         <v>100</v>
       </c>
@@ -2675,10 +2684,10 @@
       <c r="C63" t="s">
         <v>103</v>
       </c>
-      <c r="D63" s="58" t="s">
+      <c r="D63" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="E63" s="58">
+      <c r="E63" s="48">
         <v>1</v>
       </c>
       <c r="F63" s="38" t="s">
@@ -2704,8 +2713,8 @@
       <c r="C64" t="s">
         <v>103</v>
       </c>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="48"/>
       <c r="F64" s="38" t="s">
         <v>110</v>
       </c>
@@ -2729,8 +2738,8 @@
       <c r="C65" t="s">
         <v>103</v>
       </c>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
       <c r="F65" s="38" t="s">
         <v>110</v>
       </c>
@@ -2754,8 +2763,8 @@
       <c r="C66" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="58"/>
-      <c r="E66" s="58"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="48"/>
       <c r="F66" s="38" t="s">
         <v>110</v>
       </c>
@@ -2779,8 +2788,8 @@
       <c r="C67" t="s">
         <v>103</v>
       </c>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
       <c r="F67" s="38" t="s">
         <v>110</v>
       </c>
@@ -2804,8 +2813,8 @@
       <c r="C68" t="s">
         <v>103</v>
       </c>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
       <c r="F68" s="38" t="s">
         <v>110</v>
       </c>
@@ -2829,8 +2838,8 @@
       <c r="C69" t="s">
         <v>103</v>
       </c>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
       <c r="F69" s="38" t="s">
         <v>110</v>
       </c>
@@ -2854,8 +2863,8 @@
       <c r="C70" t="s">
         <v>103</v>
       </c>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
       <c r="F70" s="38" t="s">
         <v>110</v>
       </c>
@@ -2879,8 +2888,8 @@
       <c r="C71" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
       <c r="F71" s="38" t="s">
         <v>110</v>
       </c>
@@ -2941,26 +2950,33 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="C74" s="45"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="42"/>
+      <c r="A74" s="15">
+        <v>74</v>
+      </c>
+      <c r="C74" s="45">
+        <v>43210</v>
+      </c>
+      <c r="D74" t="s">
+        <v>131</v>
+      </c>
+      <c r="E74" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="G74" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="H74" t="s">
+        <v>39</v>
+      </c>
+      <c r="I74" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D63:D71"/>
-    <mergeCell ref="E63:E71"/>
-    <mergeCell ref="G2:G16"/>
-    <mergeCell ref="H2:H16"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
-    <mergeCell ref="F19:F34"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="F2:F16"/>
     <mergeCell ref="K19:K34"/>
     <mergeCell ref="F35:F59"/>
     <mergeCell ref="G35:G59"/>
@@ -2971,6 +2987,19 @@
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
     <mergeCell ref="J19:J34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
+    <mergeCell ref="F19:F34"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="F2:F16"/>
+    <mergeCell ref="D63:D71"/>
+    <mergeCell ref="E63:E71"/>
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="H2:H16"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Review about SRS_V_2.0
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.1.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="139">
   <si>
     <t>Review Log</t>
   </si>
@@ -508,6 +508,12 @@
   </si>
   <si>
     <t xml:space="preserve">need to change title </t>
+  </si>
+  <si>
+    <t>poor details in this section and not understandable, you have to mention at less the sequence</t>
+  </si>
+  <si>
+    <t>REQ2.2.8</t>
   </si>
 </sst>
 </file>
@@ -743,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -874,12 +880,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -906,6 +906,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,7 +979,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1002,7 +1014,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1211,11 +1223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,29 +1279,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>1.2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="59">
         <v>2</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="59" t="s">
         <v>108</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -1307,12 +1319,12 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1328,12 +1340,12 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1349,12 +1361,12 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1370,12 +1382,12 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1391,12 +1403,12 @@
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1405,19 +1417,19 @@
       </c>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
       <c r="I8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1433,12 +1445,12 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
       <c r="I9" s="16" t="s">
         <v>26</v>
       </c>
@@ -1452,12 +1464,12 @@
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
       <c r="I10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1473,12 +1485,12 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1494,12 +1506,12 @@
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
       <c r="I12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1515,12 +1527,12 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
       <c r="I13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1536,12 +1548,12 @@
       <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
       <c r="I14" s="7" t="s">
         <v>35</v>
       </c>
@@ -1557,12 +1569,12 @@
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
       <c r="I15" s="24" t="s">
         <v>40</v>
       </c>
@@ -1578,12 +1590,12 @@
       <c r="B16" s="7">
         <v>2.5</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="24" t="s">
         <v>42</v>
       </c>
@@ -1661,31 +1673,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="59">
         <v>1</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="59" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="49" t="s">
+      <c r="J19" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="52" t="s">
+      <c r="K19" s="50" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1694,17 +1706,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="53"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="51"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -1713,17 +1725,17 @@
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="53"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="51"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -1732,17 +1744,17 @@
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="50"/>
-      <c r="K22" s="53"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="51"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -1751,17 +1763,17 @@
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="50"/>
-      <c r="K23" s="53"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1770,17 +1782,17 @@
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="50"/>
-      <c r="K24" s="53"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="51"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1789,17 +1801,17 @@
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="50"/>
-      <c r="K25" s="53"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="51"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1808,34 +1820,34 @@
       <c r="B26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="50"/>
-      <c r="K26" s="53"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="51"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="50"/>
-      <c r="K27" s="53"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="51"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1844,17 +1856,17 @@
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="50"/>
-      <c r="K28" s="53"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="51"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1863,17 +1875,17 @@
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="50"/>
-      <c r="K29" s="53"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="51"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1882,17 +1894,17 @@
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="50"/>
-      <c r="K30" s="53"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="51"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -1901,17 +1913,17 @@
       <c r="B31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="53"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="51"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -1920,17 +1932,17 @@
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
       <c r="I32" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="50"/>
-      <c r="K32" s="53"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="51"/>
     </row>
     <row r="33" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1939,17 +1951,17 @@
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
       <c r="I33" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="J33" s="50"/>
-      <c r="K33" s="53"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="51"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
@@ -1958,17 +1970,17 @@
       <c r="B34" s="7">
         <v>6.2</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
       <c r="I34" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="51"/>
-      <c r="K34" s="54"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="52"/>
     </row>
     <row r="35" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31">
@@ -1977,20 +1989,20 @@
       <c r="B35" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D35" s="56" t="s">
         <v>69</v>
       </c>
       <c r="E35" s="11"/>
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="55" t="s">
+      <c r="G35" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="49" t="s">
+      <c r="H35" s="59" t="s">
         <v>71</v>
       </c>
       <c r="I35" s="33" t="s">
@@ -2010,12 +2022,12 @@
       <c r="B36" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="56"/>
-      <c r="D36" s="59"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="50"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="60"/>
       <c r="I36" s="33" t="s">
         <v>76</v>
       </c>
@@ -2033,12 +2045,12 @@
       <c r="B37" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="59"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="57"/>
       <c r="E37" s="13"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="50"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="33" t="s">
         <v>73</v>
       </c>
@@ -2059,12 +2071,12 @@
       <c r="B38" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="59"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="57"/>
       <c r="E38" s="13"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="50"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="60"/>
       <c r="I38" s="33" t="s">
         <v>74</v>
       </c>
@@ -2082,12 +2094,12 @@
       <c r="B39" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="59"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="50"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="60"/>
       <c r="I39" s="33" t="s">
         <v>73</v>
       </c>
@@ -2105,12 +2117,12 @@
       <c r="B40" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="D40" s="59"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="57"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="50"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="60"/>
       <c r="I40" s="33" t="s">
         <v>74</v>
       </c>
@@ -2131,12 +2143,12 @@
       <c r="B41" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="59"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="57"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="50"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="60"/>
       <c r="I41" s="33" t="s">
         <v>73</v>
       </c>
@@ -2154,12 +2166,12 @@
       <c r="B42" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="D42" s="59"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="57"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="50"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="60"/>
       <c r="I42" s="33" t="s">
         <v>79</v>
       </c>
@@ -2180,12 +2192,12 @@
       <c r="B43" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="D43" s="59"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="57"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="50"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="60"/>
       <c r="I43" s="33" t="s">
         <v>81</v>
       </c>
@@ -2203,12 +2215,12 @@
       <c r="B44" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="56"/>
-      <c r="D44" s="59"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="57"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="50"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="60"/>
       <c r="I44" s="33" t="s">
         <v>73</v>
       </c>
@@ -2229,12 +2241,12 @@
       <c r="B45" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="59"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="57"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="50"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="60"/>
       <c r="I45" s="33" t="s">
         <v>79</v>
       </c>
@@ -2255,12 +2267,12 @@
       <c r="B46" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="56"/>
-      <c r="D46" s="59"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="57"/>
       <c r="E46" s="13"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="50"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="60"/>
       <c r="I46" s="33" t="s">
         <v>81</v>
       </c>
@@ -2278,12 +2290,12 @@
       <c r="B47" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="56"/>
-      <c r="D47" s="59"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="57"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="50"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="60"/>
       <c r="I47" s="33" t="s">
         <v>73</v>
       </c>
@@ -2304,12 +2316,12 @@
       <c r="B48" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="56"/>
-      <c r="D48" s="59"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="57"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="50"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="60"/>
       <c r="I48" s="33" t="s">
         <v>79</v>
       </c>
@@ -2330,12 +2342,12 @@
       <c r="B49" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="56"/>
-      <c r="D49" s="59"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="57"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="50"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="60"/>
       <c r="I49" s="33" t="s">
         <v>73</v>
       </c>
@@ -2353,12 +2365,12 @@
       <c r="B50" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="56"/>
-      <c r="D50" s="59"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="57"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="50"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="60"/>
       <c r="I50" s="33" t="s">
         <v>73</v>
       </c>
@@ -2379,12 +2391,12 @@
       <c r="B51" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="59"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="57"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="50"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="60"/>
       <c r="I51" s="33" t="s">
         <v>79</v>
       </c>
@@ -2402,12 +2414,12 @@
       <c r="B52" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="56"/>
-      <c r="D52" s="59"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="57"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="50"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="60"/>
       <c r="I52" s="33" t="s">
         <v>81</v>
       </c>
@@ -2425,12 +2437,12 @@
       <c r="B53" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="56"/>
-      <c r="D53" s="59"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="57"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="50"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="60"/>
       <c r="I53" s="33" t="s">
         <v>73</v>
       </c>
@@ -2451,12 +2463,12 @@
       <c r="B54" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="56"/>
-      <c r="D54" s="59"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="50"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="60"/>
       <c r="I54" s="33" t="s">
         <v>79</v>
       </c>
@@ -2477,12 +2489,12 @@
       <c r="B55" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="59"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="57"/>
       <c r="E55" s="13"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="50"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="60"/>
       <c r="I55" s="33" t="s">
         <v>87</v>
       </c>
@@ -2500,12 +2512,12 @@
       <c r="B56" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="59"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="57"/>
       <c r="E56" s="13"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="50"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="60"/>
       <c r="I56" s="33" t="s">
         <v>89</v>
       </c>
@@ -2526,12 +2538,12 @@
       <c r="B57" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="56"/>
-      <c r="D57" s="59"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="57"/>
       <c r="E57" s="13"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
-      <c r="H57" s="50"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="60"/>
       <c r="I57" s="34" t="s">
         <v>89</v>
       </c>
@@ -2549,12 +2561,12 @@
       <c r="B58" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="56"/>
-      <c r="D58" s="59"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="57"/>
       <c r="E58" s="13"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="50"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="60"/>
       <c r="I58" s="36" t="s">
         <v>101</v>
       </c>
@@ -2572,12 +2584,12 @@
       <c r="B59" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="57"/>
-      <c r="D59" s="60"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="18"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="57"/>
-      <c r="H59" s="51"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="61"/>
       <c r="I59" s="36" t="s">
         <v>101</v>
       </c>
@@ -2598,10 +2610,10 @@
       <c r="C60" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="49" t="s">
+      <c r="D60" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="59" t="s">
         <v>99</v>
       </c>
       <c r="F60" s="29" t="s">
@@ -2629,8 +2641,8 @@
       <c r="C61" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="29" t="s">
         <v>100</v>
       </c>
@@ -2684,10 +2696,10 @@
       <c r="C63" t="s">
         <v>103</v>
       </c>
-      <c r="D63" s="48" t="s">
+      <c r="D63" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="E63" s="48">
+      <c r="E63" s="62">
         <v>1</v>
       </c>
       <c r="F63" s="38" t="s">
@@ -2713,8 +2725,8 @@
       <c r="C64" t="s">
         <v>103</v>
       </c>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
       <c r="F64" s="38" t="s">
         <v>110</v>
       </c>
@@ -2738,8 +2750,8 @@
       <c r="C65" t="s">
         <v>103</v>
       </c>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
       <c r="F65" s="38" t="s">
         <v>110</v>
       </c>
@@ -2763,8 +2775,8 @@
       <c r="C66" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
       <c r="F66" s="38" t="s">
         <v>110</v>
       </c>
@@ -2788,8 +2800,8 @@
       <c r="C67" t="s">
         <v>103</v>
       </c>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
       <c r="F67" s="38" t="s">
         <v>110</v>
       </c>
@@ -2813,8 +2825,8 @@
       <c r="C68" t="s">
         <v>103</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
       <c r="F68" s="38" t="s">
         <v>110</v>
       </c>
@@ -2838,8 +2850,8 @@
       <c r="C69" t="s">
         <v>103</v>
       </c>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
       <c r="F69" s="38" t="s">
         <v>110</v>
       </c>
@@ -2863,8 +2875,8 @@
       <c r="C70" t="s">
         <v>103</v>
       </c>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="62"/>
       <c r="F70" s="38" t="s">
         <v>110</v>
       </c>
@@ -2888,8 +2900,8 @@
       <c r="C71" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
       <c r="F71" s="38" t="s">
         <v>110</v>
       </c>
@@ -2949,7 +2961,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>74</v>
       </c>
@@ -2975,8 +2987,50 @@
         <v>136</v>
       </c>
     </row>
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="45">
+        <v>43210</v>
+      </c>
+      <c r="D75" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F75" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G75" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="H75" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I75" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D63:D71"/>
+    <mergeCell ref="E63:E71"/>
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="H2:H16"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
+    <mergeCell ref="F19:F34"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="F2:F16"/>
     <mergeCell ref="K19:K34"/>
     <mergeCell ref="F35:F59"/>
     <mergeCell ref="G35:G59"/>
@@ -2987,19 +3041,6 @@
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
     <mergeCell ref="J19:J34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
-    <mergeCell ref="F19:F34"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="F2:F16"/>
-    <mergeCell ref="D63:D71"/>
-    <mergeCell ref="E63:E71"/>
-    <mergeCell ref="G2:G16"/>
-    <mergeCell ref="H2:H16"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>